<commit_message>
Time Series Decompositon Practise1
</commit_message>
<xml_diff>
--- a/EVDS.xlsx
+++ b/EVDS.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Serpil Veri Bilimi\Zaman Serileri\Ayrıştırma-1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C027C32E-A59E-43F0-9179-8AF7551C990B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="23040" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EVDS" sheetId="1" r:id="rId4"/>
+    <sheet name="EVDS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Tarih</t>
   </si>
@@ -323,23 +328,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -350,34 +347,39 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -667,19 +669,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -695,7 +694,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -703,7 +702,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -711,55 +710,55 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>911.66666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>911.66666666667004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>578.33333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>578.33333333332996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>1116.6666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>1116.6666666666999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>2617.6666666667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>2617.6666666667002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>1124.3333333333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1124.3333333333001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>683.33333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>683.33333333332996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -767,23 +766,23 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>3096.3333333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3096.3333333332998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>1289.3333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>1289.3333333333001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -791,7 +790,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -799,47 +798,47 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>2776.3333333333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>2776.3333333332998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>1076.6666666667</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>1076.6666666666999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>741.66666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>741.66666666667004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1321.6666666667</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>1321.6666666666999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="2">
-        <v>3056.3333333333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>3056.3333333332998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -847,87 +846,87 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>957.33333333333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>957.33333333332996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="2">
-        <v>1694.3333333333</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>1694.3333333333001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>3540.3333333333</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>3540.3333333332998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="2">
-        <v>1596.3333333333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>1596.3333333333001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="2">
-        <v>856.33333333333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>856.33333333332996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="2">
-        <v>1556.6666666667</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>1556.6666666666999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="2">
-        <v>3402.6666666667</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>3402.6666666667002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="2">
-        <v>1844.3333333333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>1844.3333333333001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="2">
-        <v>849.33333333333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>849.33333333332996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="2">
-        <v>1667.6666666667</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>1667.6666666666999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -935,55 +934,55 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="2">
-        <v>1918.3333333333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>1918.3333333333001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="2">
-        <v>1085.6666666667</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>1085.6666666666999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="2">
-        <v>1969.6666666667</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>1969.6666666666999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2">
-        <v>3388.6666666667</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>3388.6666666667002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="2">
-        <v>1907.3333333333</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>1907.3333333333001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="2">
-        <v>1008.6666666667</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>1008.6666666667001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -991,23 +990,23 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="2">
-        <v>3326.6666666667</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>3326.6666666667002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="2">
-        <v>2221.3333333333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>2221.3333333332998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1023,31 +1022,31 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="2">
-        <v>3468.6666666667</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>3468.6666666667002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="2">
-        <v>2290.3333333333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>2290.3333333332998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="2">
-        <v>1369.3333333333</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>1369.3333333333001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1063,15 +1062,15 @@
         <v>3868</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="2">
-        <v>2222.3333333333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>2222.3333333332998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>3619</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1119,31 +1118,31 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="2">
-        <v>2405.6666666667</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>2405.6666666667002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="2">
-        <v>1387.3333333333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>1387.3333333333001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="2">
-        <v>947.33333333333</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>947.33333333332996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1151,15 +1150,15 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="2">
-        <v>3369.6666666667</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>3369.6666666667002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1167,23 +1166,23 @@
         <v>1765</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="2">
-        <v>1234.6666666667</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>1234.6666666666999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="2">
-        <v>2065.3333333333</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>2065.3333333332998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1191,31 +1190,31 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="2">
-        <v>1892.6666666667</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>1892.6666666666999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" s="2">
-        <v>1485.6666666667</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>1485.6666666666999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="2">
-        <v>2731.6666666667</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>2731.6666666667002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1223,15 +1222,15 @@
         <v>4614</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="2">
-        <v>2603.6666666667</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>2603.6666666667002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1247,55 +1246,55 @@
         <v>791</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" s="2">
-        <v>1510.3333333333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>1510.3333333333001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="2">
-        <v>1280.3333333333</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>1280.3333333333001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="2">
-        <v>815.66666666667</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>815.66666666667004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="2">
-        <v>1257.6666666667</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>1257.6666666666999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="2">
-        <v>4087.3333333333</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>4087.3333333332998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="2">
-        <v>2717.3333333333</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>2717.3333333332998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -1303,23 +1302,23 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="2">
-        <v>3226.3333333333</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>3226.3333333332998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" s="2">
-        <v>5228.6666666667</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>5228.6666666666997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>3370</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -1335,36 +1334,36 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="2">
-        <v>3784.3333333333</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>3784.3333333332998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" s="2">
-        <v>5950.3333333333</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>5950.3333333333003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85" s="2">
-        <v>3621.6666666667</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>3621.6666666667002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -1375,12 +1374,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>93</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>97</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>99</v>
       </c>
@@ -1424,17 +1423,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>